<commit_message>
docs: Modify dice loss to dice score
Modify dice loss to dice score in lr recode sheet
And add grid search sequence sheet
</commit_message>
<xml_diff>
--- a/Learning record sheet.xlsx
+++ b/Learning record sheet.xlsx
@@ -19,10 +19,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <x:si>
     <x:r>
-      <x:t xml:space="preserve">원본 데이터 = Case 2
+      <x:t xml:space="preserve">Dice Score (test)
+</x:t>
+    </x:r>
+    <x:r>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+          <x:rPr hs:extension="1">
+            <x:rFont val="맑은 고딕"/>
+            <x:sz val="7"/>
+            <x:color rgb="ffbfbfbf"/>
+            <x:b val="1"/>
+            <hs:size val="100"/>
+            <hs:ratio val="100"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:rPr>
+        </mc:Choice>
+        <mc:Fallback>
+          <x:rPr>
+            <x:rFont val="맑은 고딕"/>
+            <x:sz val="7"/>
+            <x:color rgb="ffbfbfbf"/>
+            <x:b val="1"/>
+          </x:rPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
+      <x:t>동일 테스트셋 10번 테스트 평균값</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:t xml:space="preserve">[Double] 복합 데이터 증강
 </x:t>
     </x:r>
     <x:r>
@@ -50,15 +81,6 @@
       </mc:AlternateContent>
       <x:t>(Batch size = 64)</x:t>
     </x:r>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 3</x:t>
   </x:si>
   <x:si>
     <x:r>
@@ -102,7 +124,7 @@
           <x:rPr hs:extension="1">
             <x:rFont val="맑은 고딕"/>
             <x:sz val="7"/>
-            <x:color rgb="ffbfbfbf"/>
+            <x:color rgb="ffffffff"/>
             <x:b val="1"/>
             <hs:size val="100"/>
             <hs:ratio val="100"/>
@@ -114,7 +136,7 @@
           <x:rPr>
             <x:rFont val="맑은 고딕"/>
             <x:sz val="7"/>
-            <x:color rgb="ffbfbfbf"/>
+            <x:color rgb="ffffffff"/>
             <x:b val="1"/>
           </x:rPr>
         </mc:Fallback>
@@ -123,8 +145,32 @@
     </x:r>
   </x:si>
   <x:si>
+    <x:t>Case 1 
+(1:1 비율 변환)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Original + Case 1 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>[이미지 사이즈]
+224 * 224</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 
+(중앙점 평행 이동)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 4</x:t>
+  </x:si>
+  <x:si>
     <x:r>
-      <x:t xml:space="preserve">[Double] 복합 데이터 증강
+      <x:t xml:space="preserve">모든 데이터 중앙 평행이동
 </x:t>
     </x:r>
     <x:r>
@@ -152,43 +198,6 @@
       </mc:AlternateContent>
       <x:t>(Batch size = 64)</x:t>
     </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">dice loss (test)
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="7"/>
-            <x:color rgb="ffffffff"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="7"/>
-            <x:color rgb="ffffffff"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>동일 테스트셋 10번 테스트 평균값</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2 + Case 3</x:t>
   </x:si>
   <x:si>
     <x:r>
@@ -253,37 +262,127 @@
     </x:r>
   </x:si>
   <x:si>
+    <x:t>Original + Case 1 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 1 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
     <x:t>Original + Case 2 + Case 3 + Case 4</x:t>
   </x:si>
   <x:si>
     <x:t>Original + Case 1 + Case 2 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Blue == 2nd (2 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Red == 1st (3 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Green == 3rd (1 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>best dice loss (train)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Best Dice Score (train)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Best Dice Score (val)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>best dice loss (val)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2nd Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>train lr std</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1st Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3rd Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 1</x:t>
   </x:si>
   <x:si>
     <x:t>Case 4 
 (데이터들의 최대 길이 대비 축소 비율의 평균값으로
-가로/세로 비율 고정, 크기 변환)</x:t>
+크기 변환, 가로/세로 비율 고정)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2 + Case 3</x:t>
   </x:si>
   <x:si>
     <x:t>Original + Case 2 + Case 4</x:t>
   </x:si>
   <x:si>
-    <x:t>Original + Case 2 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2</x:t>
+    <x:t>Case 2 + Case 1 + Case 4</x:t>
   </x:si>
   <x:si>
     <x:t>Case 3
 (비율 고정, 최대 크기 변환)</x:t>
   </x:si>
   <x:si>
+    <x:t>Original + Case 1 + Case 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2  + Case 1 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 3</x:t>
+  </x:si>
+  <x:si>
     <x:t>Original + Case 3 + Case 4</x:t>
   </x:si>
   <x:si>
     <x:t>Original + Case 1 + Case 4</x:t>
   </x:si>
   <x:si>
-    <x:t>Original + Case 1 + Case 3</x:t>
+    <x:t>12 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original</x:t>
+  </x:si>
+  <x:si>
+    <x:t>val lr std</x:t>
   </x:si>
   <x:si>
     <x:r>
@@ -317,104 +416,15 @@
     </x:r>
   </x:si>
   <x:si>
-    <x:t>Original + Case 1 + Case 2 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2nd Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1st Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>train lr std</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3rd Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 
-(중앙점 평행 이동)</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Original + Case 1 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 1 
-(1:1 비율 변환)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[이미지 사이즈]
-224 * 224</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>best dice loss (train)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>best dice loss (val)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Green == 3rd (1 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Red == 1st (3 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blue == 2nd (2 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>val lr std</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1번 서버</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2  + Case 1 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1 + Case 4</x:t>
+    <x:t>Grid Search Start
+(Dice Score (test))</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="23">
+  <x:fonts count="20">
     <x:font>
       <x:name val="맑은 고딕"/>
       <x:sz val="11"/>
@@ -468,28 +478,12 @@
       <x:color rgb="ffff0000"/>
       <x:b val="1"/>
     </x:font>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff6182d6"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff6182d6"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff6182d6"/>
+      <x:b val="1"/>
+    </x:font>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:font hs:extension="1">
@@ -572,12 +566,6 @@
         </x:font>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:font>
-      <x:name val="맑은 고딕"/>
-      <x:sz val="13"/>
-      <x:color rgb="ffffffff"/>
-      <x:b val="1"/>
-    </x:font>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:font hs:extension="1">
@@ -602,51 +590,7 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:font hs:extension="1">
           <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff289b6e"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff289b6e"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff6182d6"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ff6182d6"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
+          <x:sz val="13"/>
           <x:color rgb="ffffffff"/>
           <x:b val="1"/>
           <hs:size val="100"/>
@@ -658,8 +602,30 @@
       <mc:Fallback>
         <x:font>
           <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
+          <x:sz val="13"/>
           <x:color rgb="ffffffff"/>
+          <x:b val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="7"/>
+          <x:color rgb="ffbfbfbf"/>
+          <x:b val="1"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="7"/>
+          <x:color rgb="ffbfbfbf"/>
           <x:b val="1"/>
         </x:font>
       </mc:Fallback>
@@ -681,28 +647,6 @@
         <x:font>
           <x:name val="맑은 고딕"/>
           <x:sz val="8"/>
-          <x:color rgb="ffbfbfbf"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="7"/>
-          <x:color rgb="ffbfbfbf"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="7"/>
           <x:color rgb="ffbfbfbf"/>
           <x:b val="1"/>
         </x:font>
@@ -763,7 +707,7 @@
       </x:patternFill>
     </x:fill>
   </x:fills>
-  <x:borders count="9">
+  <x:borders count="12">
     <x:border>
       <x:left>
         <x:color rgb="ff000000"/>
@@ -890,6 +834,48 @@
         <x:color rgb="ff67530e"/>
       </x:bottom>
     </x:border>
+    <x:border>
+      <x:left style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:left>
+      <x:right style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:right>
+      <x:top style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:left>
+      <x:right style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:right>
+      <x:top>
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:left>
+      <x:right style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:right>
+      <x:top>
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom style="thick">
+        <x:color rgb="ffff0000"/>
+      </x:bottom>
+    </x:border>
   </x:borders>
   <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -899,7 +885,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="52">
+  <x:cellXfs count="69">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -1093,19 +1079,6 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -1135,6 +1108,308 @@
     </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -1148,13 +1423,13 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1174,26 +1449,65 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1213,45 +1527,6 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -1265,234 +1540,166 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
         </x:xf>
       </mc:Choice>
       <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+        <x:xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
         </x:xf>
       </mc:Choice>
       <mc:Fallback>
-        <x:xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -1903,7 +2110,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1933,8 +2140,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17764124" y="634999"/>
-          <a:ext cx="4683125" cy="3667124"/>
+          <a:off x="17757322" y="625928"/>
+          <a:ext cx="4680857" cy="3673928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2259,10 +2466,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:K57"/>
+  <x:dimension ref="A1:K62"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="60" zoomScaleNormal="80" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <x:selection activeCell="A1" activeCellId="0" sqref="A1:A3"/>
+    <x:sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <x:selection activeCell="C23" activeCellId="0" sqref="C23:C23"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
@@ -2280,105 +2487,105 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:11">
-      <x:c r="A1" s="40" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="B1" s="33" t="s">
-        <x:v>43</x:v>
+      <x:c r="A1" s="57" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B1" s="31" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C1" s="3"/>
       <x:c r="D1" s="3"/>
       <x:c r="E1" s="3"/>
       <x:c r="F1" s="3"/>
-      <x:c r="G1" s="20"/>
-      <x:c r="H1" s="20"/>
-      <x:c r="I1" s="42"/>
-      <x:c r="J1" s="42"/>
-      <x:c r="K1" s="42"/>
+      <x:c r="G1" s="19"/>
+      <x:c r="H1" s="19"/>
+      <x:c r="I1" s="19"/>
+      <x:c r="J1" s="19"/>
+      <x:c r="K1" s="19"/>
     </x:row>
     <x:row r="2" spans="1:11">
-      <x:c r="A2" s="41"/>
-      <x:c r="B2" s="32" t="s">
-        <x:v>44</x:v>
+      <x:c r="A2" s="58"/>
+      <x:c r="B2" s="30" t="s">
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C2" s="3"/>
       <x:c r="D2" s="3"/>
       <x:c r="E2" s="3"/>
       <x:c r="F2" s="3"/>
-      <x:c r="G2" s="20"/>
-      <x:c r="H2" s="20"/>
-      <x:c r="I2" s="42"/>
-      <x:c r="J2" s="42"/>
-      <x:c r="K2" s="42"/>
+      <x:c r="G2" s="19"/>
+      <x:c r="H2" s="19"/>
+      <x:c r="I2" s="19"/>
+      <x:c r="J2" s="19"/>
+      <x:c r="K2" s="19"/>
     </x:row>
     <x:row r="3" spans="1:11">
-      <x:c r="A3" s="41"/>
-      <x:c r="B3" s="31" t="s">
-        <x:v>42</x:v>
+      <x:c r="A3" s="58"/>
+      <x:c r="B3" s="29" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C3" s="3"/>
       <x:c r="D3" s="3"/>
       <x:c r="E3" s="3"/>
       <x:c r="F3" s="3"/>
-      <x:c r="G3" s="20"/>
-      <x:c r="H3" s="20"/>
-      <x:c r="I3" s="42"/>
-      <x:c r="J3" s="42"/>
-      <x:c r="K3" s="42"/>
+      <x:c r="G3" s="19"/>
+      <x:c r="H3" s="19"/>
+      <x:c r="I3" s="19"/>
+      <x:c r="J3" s="19"/>
+      <x:c r="K3" s="19"/>
     </x:row>
     <x:row r="4" spans="1:11" ht="55.5" customHeight="1">
-      <x:c r="A4" s="43"/>
+      <x:c r="A4" s="59"/>
       <x:c r="B4" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C4" s="6" t="s">
-        <x:v>46</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D4" s="6" t="s">
-        <x:v>36</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E4" s="6" t="s">
-        <x:v>34</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F4" s="6" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G4" s="17" t="s">
-        <x:v>14</x:v>
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="G4" s="56" t="s">
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H4"/>
-      <x:c r="I4" s="42"/>
-      <x:c r="J4" s="42"/>
-      <x:c r="K4" s="42"/>
+      <x:c r="I4" s="19"/>
+      <x:c r="J4" s="19"/>
+      <x:c r="K4" s="19"/>
     </x:row>
     <x:row r="5" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A5" s="43"/>
-      <x:c r="B5" s="39" t="s">
-        <x:v>5</x:v>
+      <x:c r="A5" s="59"/>
+      <x:c r="B5" s="8" t="s">
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C5" s="9">
-        <x:v>0.1305</x:v>
+        <x:v>0.86950000000000005</x:v>
       </x:c>
       <x:c r="D5" s="9">
-        <x:v>0.13769999999999999</x:v>
+        <x:v>0.86229999999999996</x:v>
       </x:c>
       <x:c r="E5" s="9">
-        <x:v>0.15570000000000001</x:v>
+        <x:v>0.84430000000000005</x:v>
       </x:c>
       <x:c r="F5" s="9">
-        <x:v>0.1744</x:v>
+        <x:v>0.8256</x:v>
       </x:c>
       <x:c r="G5" s="10">
-        <x:v>0.14410000000000001</x:v>
-      </x:c>
-      <x:c r="I5" s="42"/>
-      <x:c r="J5" s="42"/>
-      <x:c r="K5" s="42"/>
+        <x:v>0.85589999999999999</x:v>
+      </x:c>
+      <x:c r="I5" s="19"/>
+      <x:c r="J5" s="19"/>
+      <x:c r="K5" s="19"/>
     </x:row>
     <x:row r="6" spans="1:11">
-      <x:c r="A6" s="43"/>
+      <x:c r="A6" s="59"/>
       <x:c r="B6" s="11" t="s">
-        <x:v>40</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C6" s="12">
         <x:v>0.096600000000000008</x:v>
@@ -2395,14 +2602,14 @@
       <x:c r="G6" s="15">
         <x:v>0.1012</x:v>
       </x:c>
-      <x:c r="I6" s="42"/>
-      <x:c r="J6" s="42"/>
-      <x:c r="K6" s="42"/>
+      <x:c r="I6" s="19"/>
+      <x:c r="J6" s="19"/>
+      <x:c r="K6" s="19"/>
     </x:row>
     <x:row r="7" spans="1:11">
-      <x:c r="A7" s="43"/>
+      <x:c r="A7" s="59"/>
       <x:c r="B7" s="11" t="s">
-        <x:v>41</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C7" s="12">
         <x:v>0.1231</x:v>
@@ -2419,14 +2626,14 @@
       <x:c r="G7" s="15">
         <x:v>0.13719999999999999</x:v>
       </x:c>
-      <x:c r="I7" s="42"/>
-      <x:c r="J7" s="42"/>
-      <x:c r="K7" s="42"/>
+      <x:c r="I7" s="19"/>
+      <x:c r="J7" s="19"/>
+      <x:c r="K7" s="19"/>
     </x:row>
     <x:row r="8" spans="1:11">
-      <x:c r="A8" s="43"/>
+      <x:c r="A8" s="59"/>
       <x:c r="B8" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C8" s="12">
         <x:v>0.21510000000000001</x:v>
@@ -2443,14 +2650,14 @@
       <x:c r="G8" s="15">
         <x:v>0.1226</x:v>
       </x:c>
-      <x:c r="I8" s="42"/>
-      <x:c r="J8" s="42"/>
-      <x:c r="K8" s="42"/>
+      <x:c r="I8" s="19"/>
+      <x:c r="J8" s="19"/>
+      <x:c r="K8" s="19"/>
     </x:row>
     <x:row r="9" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A9" s="43"/>
+      <x:c r="A9" s="59"/>
       <x:c r="B9" s="13" t="s">
-        <x:v>45</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C9" s="14">
         <x:v>0.2475</x:v>
@@ -2467,102 +2674,104 @@
       <x:c r="G9" s="16">
         <x:v>0.20000000000000001</x:v>
       </x:c>
-      <x:c r="I9" s="42"/>
-      <x:c r="J9" s="42"/>
-      <x:c r="K9" s="42"/>
+      <x:c r="I9" s="19"/>
+      <x:c r="J9" s="19"/>
+      <x:c r="K9" s="19"/>
     </x:row>
     <x:row r="10" spans="1:11">
-      <x:c r="A10" s="42"/>
+      <x:c r="A10" s="60"/>
       <x:c r="B10" s="3"/>
-      <x:c r="C10" s="20"/>
-      <x:c r="D10" s="20"/>
+      <x:c r="C10" s="19"/>
+      <x:c r="D10" s="19"/>
       <x:c r="E10" s="3"/>
-      <x:c r="F10" s="20"/>
-      <x:c r="G10" s="20"/>
-      <x:c r="H10" s="20"/>
-      <x:c r="I10" s="42"/>
-      <x:c r="J10" s="42"/>
-      <x:c r="K10" s="42"/>
+      <x:c r="F10" s="19"/>
+      <x:c r="G10" s="19"/>
+      <x:c r="H10" s="19"/>
+      <x:c r="I10" s="19"/>
+      <x:c r="J10" s="19"/>
+      <x:c r="K10" s="19"/>
     </x:row>
     <x:row r="11" spans="1:11">
-      <x:c r="A11" s="42"/>
-      <x:c r="B11" s="20"/>
-      <x:c r="C11" s="20"/>
-      <x:c r="D11" s="20"/>
+      <x:c r="A11" s="60"/>
+      <x:c r="B11" s="68" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C11" s="19"/>
+      <x:c r="D11" s="19"/>
       <x:c r="E11" s="3"/>
-      <x:c r="F11" s="20"/>
-      <x:c r="G11" s="20"/>
-      <x:c r="H11" s="20"/>
-      <x:c r="I11" s="42"/>
-      <x:c r="J11" s="42"/>
-      <x:c r="K11" s="42"/>
+      <x:c r="F11" s="19"/>
+      <x:c r="G11" s="19"/>
+      <x:c r="H11" s="19"/>
+      <x:c r="I11" s="19"/>
+      <x:c r="J11" s="19"/>
+      <x:c r="K11" s="19"/>
     </x:row>
     <x:row r="12" spans="1:11">
-      <x:c r="A12" s="42"/>
-      <x:c r="B12" s="20"/>
-      <x:c r="C12" s="20"/>
-      <x:c r="D12" s="20"/>
+      <x:c r="A12" s="60"/>
+      <x:c r="B12" s="67"/>
+      <x:c r="C12" s="19"/>
+      <x:c r="D12" s="19"/>
       <x:c r="E12" s="3"/>
-      <x:c r="F12" s="20"/>
-      <x:c r="G12" s="20"/>
-      <x:c r="H12" s="20"/>
-      <x:c r="I12" s="42"/>
-      <x:c r="J12" s="42"/>
-      <x:c r="K12" s="42"/>
+      <x:c r="F12" s="19"/>
+      <x:c r="G12" s="19"/>
+      <x:c r="H12" s="19"/>
+      <x:c r="I12" s="19"/>
+      <x:c r="J12" s="19"/>
+      <x:c r="K12" s="19"/>
     </x:row>
     <x:row r="13" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A13" s="42"/>
+      <x:c r="A13" s="60"/>
       <x:c r="B13" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C13" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D13" s="61" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="6" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F13" s="7" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C13" s="6" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="D13" s="6" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E13" s="6" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="F13" s="7" t="s">
-        <x:v>33</x:v>
-      </x:c>
       <x:c r="G13" s="2"/>
-      <x:c r="I13" s="42"/>
-      <x:c r="J13" s="42"/>
-      <x:c r="K13" s="42"/>
+      <x:c r="I13" s="19"/>
+      <x:c r="J13" s="19"/>
+      <x:c r="K13" s="19"/>
     </x:row>
     <x:row r="14" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A14" s="42"/>
+      <x:c r="A14" s="60"/>
       <x:c r="B14" s="8" t="s">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C14" s="9">
-        <x:v>0.10879999999999999</x:v>
-      </x:c>
-      <x:c r="D14" s="9">
-        <x:v>0.1003</x:v>
+        <x:v>0.89119999999999999</x:v>
+      </x:c>
+      <x:c r="D14" s="62">
+        <x:v>0.89970000000000006</x:v>
       </x:c>
       <x:c r="E14" s="9">
-        <x:v>0.1227</x:v>
+        <x:v>0.87729999999999997</x:v>
       </x:c>
       <x:c r="F14" s="10">
-        <x:v>0.10879999999999999</x:v>
+        <x:v>0.89119999999999999</x:v>
       </x:c>
       <x:c r="G14" s="3"/>
-      <x:c r="I14" s="42"/>
-      <x:c r="J14" s="42"/>
-      <x:c r="K14" s="42"/>
+      <x:c r="I14" s="19"/>
+      <x:c r="J14" s="19"/>
+      <x:c r="K14" s="19"/>
     </x:row>
     <x:row r="15" spans="1:11">
-      <x:c r="A15" s="42"/>
+      <x:c r="A15" s="60"/>
       <x:c r="B15" s="11" t="s">
-        <x:v>40</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C15" s="12">
         <x:v>0.064600000000000002</x:v>
       </x:c>
-      <x:c r="D15" s="12">
+      <x:c r="D15" s="63">
         <x:v>0.054699999999999993</x:v>
       </x:c>
       <x:c r="E15" s="12">
@@ -2572,19 +2781,19 @@
         <x:v>0.079299999999999993</x:v>
       </x:c>
       <x:c r="G15" s="3"/>
-      <x:c r="I15" s="42"/>
-      <x:c r="J15" s="42"/>
-      <x:c r="K15" s="42"/>
+      <x:c r="I15" s="19"/>
+      <x:c r="J15" s="19"/>
+      <x:c r="K15" s="19"/>
     </x:row>
     <x:row r="16" spans="1:11">
-      <x:c r="A16" s="42"/>
+      <x:c r="A16" s="60"/>
       <x:c r="B16" s="11" t="s">
-        <x:v>41</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C16" s="12">
         <x:v>0.1027</x:v>
       </x:c>
-      <x:c r="D16" s="12">
+      <x:c r="D16" s="63">
         <x:v>0.097199999999999998</x:v>
       </x:c>
       <x:c r="E16" s="12">
@@ -2594,19 +2803,19 @@
         <x:v>0.10730000000000001</x:v>
       </x:c>
       <x:c r="G16" s="3"/>
-      <x:c r="I16" s="42"/>
-      <x:c r="J16" s="42"/>
-      <x:c r="K16" s="42"/>
+      <x:c r="I16" s="19"/>
+      <x:c r="J16" s="19"/>
+      <x:c r="K16" s="19"/>
     </x:row>
     <x:row r="17" spans="1:11">
-      <x:c r="A17" s="42"/>
+      <x:c r="A17" s="60"/>
       <x:c r="B17" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C17" s="12">
         <x:v>0.12130000000000001</x:v>
       </x:c>
-      <x:c r="D17" s="12">
+      <x:c r="D17" s="63">
         <x:v>0.14050000000000001</x:v>
       </x:c>
       <x:c r="E17" s="12">
@@ -2616,19 +2825,19 @@
         <x:v>0.1169</x:v>
       </x:c>
       <x:c r="G17" s="3"/>
-      <x:c r="I17" s="42"/>
-      <x:c r="J17" s="42"/>
-      <x:c r="K17" s="42"/>
+      <x:c r="I17" s="19"/>
+      <x:c r="J17" s="19"/>
+      <x:c r="K17" s="19"/>
     </x:row>
     <x:row r="18" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A18" s="42"/>
+      <x:c r="A18" s="60"/>
       <x:c r="B18" s="13" t="s">
-        <x:v>45</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C18" s="14">
         <x:v>0.16139999999999999</x:v>
       </x:c>
-      <x:c r="D18" s="14">
+      <x:c r="D18" s="64">
         <x:v>0.1817</x:v>
       </x:c>
       <x:c r="E18" s="14">
@@ -2638,119 +2847,119 @@
         <x:v>0.1893</x:v>
       </x:c>
       <x:c r="G18" s="3"/>
-      <x:c r="I18" s="42"/>
-      <x:c r="J18" s="42"/>
-      <x:c r="K18" s="42"/>
+      <x:c r="I18" s="19"/>
+      <x:c r="J18" s="19"/>
+      <x:c r="K18" s="19"/>
     </x:row>
     <x:row r="19" spans="1:11">
-      <x:c r="A19" s="42"/>
-      <x:c r="B19" s="20"/>
-      <x:c r="C19" s="20"/>
-      <x:c r="D19" s="20"/>
-      <x:c r="E19" s="20"/>
-      <x:c r="F19" s="20"/>
-      <x:c r="G19" s="20"/>
-      <x:c r="H19" s="20"/>
-      <x:c r="I19" s="42"/>
-      <x:c r="J19" s="42"/>
-      <x:c r="K19" s="42"/>
+      <x:c r="A19" s="60"/>
+      <x:c r="B19" s="19"/>
+      <x:c r="C19" s="19"/>
+      <x:c r="D19" s="19"/>
+      <x:c r="E19" s="19"/>
+      <x:c r="F19" s="19"/>
+      <x:c r="G19" s="19"/>
+      <x:c r="H19" s="19"/>
+      <x:c r="I19" s="19"/>
+      <x:c r="J19" s="19"/>
+      <x:c r="K19" s="19"/>
     </x:row>
     <x:row r="20" spans="1:11">
-      <x:c r="A20" s="42"/>
-      <x:c r="B20" s="20"/>
-      <x:c r="C20" s="36" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="D20" s="37" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E20" s="20"/>
-      <x:c r="F20" s="20"/>
-      <x:c r="G20" s="20"/>
-      <x:c r="H20" s="20"/>
-      <x:c r="I20" s="42"/>
-      <x:c r="J20" s="42"/>
-      <x:c r="K20" s="42"/>
+      <x:c r="A20" s="60"/>
+      <x:c r="B20" s="19"/>
+      <x:c r="C20" s="34" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="D20" s="35" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E20" s="19"/>
+      <x:c r="F20" s="19"/>
+      <x:c r="G20" s="19"/>
+      <x:c r="H20" s="19"/>
+      <x:c r="I20" s="19"/>
+      <x:c r="J20" s="19"/>
+      <x:c r="K20" s="19"/>
     </x:row>
     <x:row r="21" spans="1:11">
-      <x:c r="A21" s="42"/>
-      <x:c r="B21" s="20"/>
-      <x:c r="C21" s="34" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="D21" s="35" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="E21" s="35" t="s">
+      <x:c r="A21" s="60"/>
+      <x:c r="B21" s="19"/>
+      <x:c r="C21" s="32" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D21" s="33" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="F21" s="20"/>
-      <x:c r="G21" s="20"/>
-      <x:c r="H21" s="20"/>
-      <x:c r="I21" s="42"/>
-      <x:c r="J21" s="42"/>
-      <x:c r="K21" s="42"/>
+      <x:c r="E21" s="33" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F21" s="19"/>
+      <x:c r="G21" s="19"/>
+      <x:c r="H21" s="19"/>
+      <x:c r="I21" s="19"/>
+      <x:c r="J21" s="19"/>
+      <x:c r="K21" s="19"/>
     </x:row>
     <x:row r="22" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A22" s="42"/>
+      <x:c r="A22" s="60"/>
       <x:c r="B22" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C22" s="6" t="s">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C22" s="61" t="s">
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D22" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E22" s="6" t="s">
-        <x:v>20</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F22" s="6" t="s">
-        <x:v>16</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G22" s="6" t="s">
-        <x:v>15</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="H22" s="7" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="I22" s="42"/>
-      <x:c r="J22" s="42"/>
-      <x:c r="K22" s="42"/>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I22" s="19"/>
+      <x:c r="J22" s="19"/>
+      <x:c r="K22" s="19"/>
     </x:row>
     <x:row r="23" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A23" s="42"/>
+      <x:c r="A23" s="60"/>
       <x:c r="B23" s="8" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C23" s="21">
-        <x:v>0.095200000000000007</x:v>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C23" s="65">
+        <x:v>0.90480000000000005</x:v>
       </x:c>
       <x:c r="D23" s="9">
-        <x:v>0.1094</x:v>
-      </x:c>
-      <x:c r="E23" s="24">
-        <x:v>0.097100000000000009</x:v>
+        <x:v>0.89059999999999995</x:v>
+      </x:c>
+      <x:c r="E23" s="22">
+        <x:v>0.90290000000000004</x:v>
       </x:c>
       <x:c r="F23" s="9">
-        <x:v>0.1076</x:v>
+        <x:v>0.89239999999999997</x:v>
       </x:c>
       <x:c r="G23" s="9">
-        <x:v>0.1048</x:v>
+        <x:v>0.8952</x:v>
       </x:c>
       <x:c r="H23" s="10">
-        <x:v>0.1123</x:v>
-      </x:c>
-      <x:c r="I23" s="42"/>
-      <x:c r="J23" s="42"/>
-      <x:c r="K23" s="42"/>
+        <x:v>0.88770000000000004</x:v>
+      </x:c>
+      <x:c r="I23" s="19"/>
+      <x:c r="J23" s="19"/>
+      <x:c r="K23" s="19"/>
     </x:row>
     <x:row r="24" spans="1:11">
-      <x:c r="A24" s="42"/>
+      <x:c r="A24" s="60"/>
       <x:c r="B24" s="11" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C24" s="22">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C24" s="66">
         <x:v>0.049199999999999999</x:v>
       </x:c>
       <x:c r="D24" s="12">
@@ -2765,22 +2974,22 @@
       <x:c r="G24" s="12">
         <x:v>0.067300000000000004</x:v>
       </x:c>
-      <x:c r="H24" s="18">
+      <x:c r="H24" s="17">
         <x:v>0.058099999999999996</x:v>
       </x:c>
-      <x:c r="I24" s="42"/>
-      <x:c r="J24" s="42"/>
-      <x:c r="K24" s="42"/>
+      <x:c r="I24" s="19"/>
+      <x:c r="J24" s="19"/>
+      <x:c r="K24" s="19"/>
     </x:row>
     <x:row r="25" spans="1:11">
-      <x:c r="A25" s="42"/>
+      <x:c r="A25" s="60"/>
       <x:c r="B25" s="11" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C25" s="22">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C25" s="66">
         <x:v>0.093999999999999995</x:v>
       </x:c>
-      <x:c r="D25" s="29">
+      <x:c r="D25" s="27">
         <x:v>0.096799999999999997</x:v>
       </x:c>
       <x:c r="E25" s="12">
@@ -2792,22 +3001,22 @@
       <x:c r="G25" s="12">
         <x:v>0.097999999999999998</x:v>
       </x:c>
-      <x:c r="H25" s="18">
+      <x:c r="H25" s="17">
         <x:v>0.1076</x:v>
       </x:c>
-      <x:c r="I25" s="42"/>
-      <x:c r="J25" s="42"/>
-      <x:c r="K25" s="42"/>
+      <x:c r="I25" s="19"/>
+      <x:c r="J25" s="19"/>
+      <x:c r="K25" s="19"/>
     </x:row>
     <x:row r="26" spans="1:11">
-      <x:c r="A26" s="42"/>
+      <x:c r="A26" s="60"/>
       <x:c r="B26" s="11" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C26" s="12">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C26" s="63">
         <x:v>0.1085</x:v>
       </x:c>
-      <x:c r="D26" s="22">
+      <x:c r="D26" s="20">
         <x:v>0.082000000000000006</x:v>
       </x:c>
       <x:c r="E26" s="12">
@@ -2819,22 +3028,22 @@
       <x:c r="G26" s="12">
         <x:v>0.11020000000000001</x:v>
       </x:c>
-      <x:c r="H26" s="18">
+      <x:c r="H26" s="17">
         <x:v>0.0875</x:v>
       </x:c>
-      <x:c r="I26" s="42"/>
-      <x:c r="J26" s="42"/>
-      <x:c r="K26" s="42"/>
+      <x:c r="I26" s="19"/>
+      <x:c r="J26" s="19"/>
+      <x:c r="K26" s="19"/>
     </x:row>
     <x:row r="27" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A27" s="42"/>
+      <x:c r="A27" s="60"/>
       <x:c r="B27" s="13" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C27" s="14">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C27" s="64">
         <x:v>0.1237</x:v>
       </x:c>
-      <x:c r="D27" s="23">
+      <x:c r="D27" s="21">
         <x:v>0.1036</x:v>
       </x:c>
       <x:c r="E27" s="14">
@@ -2846,110 +3055,110 @@
       <x:c r="G27" s="14">
         <x:v>0.2109</x:v>
       </x:c>
-      <x:c r="H27" s="19">
+      <x:c r="H27" s="18">
         <x:v>0.14430000000000001</x:v>
       </x:c>
-      <x:c r="I27" s="42"/>
-      <x:c r="J27" s="42"/>
-      <x:c r="K27" s="42"/>
+      <x:c r="I27" s="19"/>
+      <x:c r="J27" s="19"/>
+      <x:c r="K27" s="19"/>
     </x:row>
     <x:row r="28" spans="1:11">
-      <x:c r="A28" s="42"/>
-      <x:c r="B28" s="20"/>
-      <x:c r="C28" s="20"/>
-      <x:c r="D28" s="20"/>
-      <x:c r="E28" s="20"/>
-      <x:c r="F28" s="20"/>
-      <x:c r="G28" s="20"/>
-      <x:c r="H28" s="20"/>
-      <x:c r="I28" s="42"/>
-      <x:c r="J28" s="42"/>
-      <x:c r="K28" s="42"/>
+      <x:c r="A28" s="60"/>
+      <x:c r="B28" s="19"/>
+      <x:c r="C28" s="19"/>
+      <x:c r="D28" s="19"/>
+      <x:c r="E28" s="19"/>
+      <x:c r="F28" s="19"/>
+      <x:c r="G28" s="19"/>
+      <x:c r="H28" s="19"/>
+      <x:c r="I28" s="19"/>
+      <x:c r="J28" s="19"/>
+      <x:c r="K28" s="19"/>
     </x:row>
     <x:row r="29" spans="1:11">
-      <x:c r="A29" s="42"/>
-      <x:c r="B29" s="20"/>
-      <x:c r="C29" s="20"/>
-      <x:c r="D29" s="20"/>
-      <x:c r="E29" s="20"/>
-      <x:c r="F29" s="20"/>
-      <x:c r="G29" s="20"/>
-      <x:c r="H29" s="20"/>
-      <x:c r="I29" s="42"/>
-      <x:c r="J29" s="42"/>
-      <x:c r="K29" s="42"/>
+      <x:c r="A29" s="60"/>
+      <x:c r="B29" s="19"/>
+      <x:c r="C29" s="19"/>
+      <x:c r="D29" s="19"/>
+      <x:c r="E29" s="19"/>
+      <x:c r="F29" s="19"/>
+      <x:c r="G29" s="19"/>
+      <x:c r="H29" s="19"/>
+      <x:c r="I29" s="19"/>
+      <x:c r="J29" s="19"/>
+      <x:c r="K29" s="19"/>
     </x:row>
     <x:row r="30" spans="1:11">
-      <x:c r="A30" s="42"/>
-      <x:c r="B30" s="20"/>
-      <x:c r="C30" s="35" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="D30" s="35" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E30" s="35" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="F30" s="35" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="G30" s="20"/>
-      <x:c r="H30" s="20"/>
-      <x:c r="I30" s="42"/>
-      <x:c r="J30" s="42"/>
-      <x:c r="K30" s="42"/>
+      <x:c r="A30" s="60"/>
+      <x:c r="B30" s="19"/>
+      <x:c r="C30" s="33" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D30" s="33" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E30" s="33" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="F30" s="33" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G30" s="19"/>
+      <x:c r="H30" s="19"/>
+      <x:c r="I30" s="19"/>
+      <x:c r="J30" s="19"/>
+      <x:c r="K30" s="19"/>
     </x:row>
     <x:row r="31" spans="1:11" ht="28.30000000000000071054" customHeight="1">
-      <x:c r="A31" s="42"/>
+      <x:c r="A31" s="60"/>
       <x:c r="B31" s="5" t="s">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C31" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D31" s="6" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E31" s="6" t="s">
-        <x:v>48</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F31" s="7" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G31" s="4"/>
       <x:c r="H31" s="4"/>
-      <x:c r="I31" s="42"/>
-      <x:c r="J31" s="42"/>
-      <x:c r="K31" s="42"/>
+      <x:c r="I31" s="19"/>
+      <x:c r="J31" s="19"/>
+      <x:c r="K31" s="19"/>
     </x:row>
     <x:row r="32" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A32" s="42"/>
+      <x:c r="A32" s="60"/>
       <x:c r="B32" s="8" t="s">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C32" s="9">
-        <x:v>0.0999</x:v>
-      </x:c>
-      <x:c r="D32" s="27">
-        <x:v>0.098999999999999999</x:v>
-      </x:c>
-      <x:c r="E32" s="45">
-        <x:v>0.10349999999999999</x:v>
+        <x:v>0.90010000000000001</x:v>
+      </x:c>
+      <x:c r="D32" s="25">
+        <x:v>0.90100000000000002</x:v>
+      </x:c>
+      <x:c r="E32" s="38">
+        <x:v>0.89649999999999996</x:v>
       </x:c>
       <x:c r="F32" s="10">
-        <x:v>0.106</x:v>
+        <x:v>0.89400000000000002</x:v>
       </x:c>
       <x:c r="G32" s="4"/>
       <x:c r="H32" s="4"/>
-      <x:c r="I32" s="42"/>
-      <x:c r="J32" s="42"/>
-      <x:c r="K32" s="42"/>
+      <x:c r="I32" s="19"/>
+      <x:c r="J32" s="19"/>
+      <x:c r="K32" s="19"/>
     </x:row>
     <x:row r="33" spans="1:11">
-      <x:c r="A33" s="42"/>
+      <x:c r="A33" s="60"/>
       <x:c r="B33" s="11" t="s">
-        <x:v>40</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C33" s="12">
         <x:v>0.064000000000000001</x:v>
@@ -2957,22 +3166,22 @@
       <x:c r="D33" s="12">
         <x:v>0.056399999999999995</x:v>
       </x:c>
-      <x:c r="E33" s="46">
+      <x:c r="E33" s="39">
         <x:v>0.053900000000000003</x:v>
       </x:c>
-      <x:c r="F33" s="28">
+      <x:c r="F33" s="26">
         <x:v>0.055200000000000005</x:v>
       </x:c>
       <x:c r="G33" s="3"/>
       <x:c r="H33" s="3"/>
-      <x:c r="I33" s="42"/>
-      <x:c r="J33" s="42"/>
-      <x:c r="K33" s="42"/>
+      <x:c r="I33" s="19"/>
+      <x:c r="J33" s="19"/>
+      <x:c r="K33" s="19"/>
     </x:row>
     <x:row r="34" spans="1:11">
-      <x:c r="A34" s="42"/>
+      <x:c r="A34" s="60"/>
       <x:c r="B34" s="11" t="s">
-        <x:v>41</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C34" s="12">
         <x:v>0.099399999999999999</x:v>
@@ -2988,14 +3197,14 @@
       </x:c>
       <x:c r="G34" s="3"/>
       <x:c r="H34" s="3"/>
-      <x:c r="I34" s="42"/>
-      <x:c r="J34" s="42"/>
-      <x:c r="K34" s="42"/>
+      <x:c r="I34" s="19"/>
+      <x:c r="J34" s="19"/>
+      <x:c r="K34" s="19"/>
     </x:row>
     <x:row r="35" spans="1:11">
-      <x:c r="A35" s="42"/>
+      <x:c r="A35" s="60"/>
       <x:c r="B35" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C35" s="12">
         <x:v>0.098299999999999998</x:v>
@@ -3003,27 +3212,27 @@
       <x:c r="D35" s="12">
         <x:v>0.0997</x:v>
       </x:c>
-      <x:c r="E35" s="47">
+      <x:c r="E35" s="40">
         <x:v>0.0745</x:v>
       </x:c>
-      <x:c r="F35" s="48">
+      <x:c r="F35" s="41">
         <x:v>0.082500000000000007</x:v>
       </x:c>
       <x:c r="G35" s="3"/>
       <x:c r="H35" s="3"/>
-      <x:c r="I35" s="42"/>
-      <x:c r="J35" s="42"/>
-      <x:c r="K35" s="42"/>
+      <x:c r="I35" s="19"/>
+      <x:c r="J35" s="19"/>
+      <x:c r="K35" s="19"/>
     </x:row>
     <x:row r="36" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A36" s="42"/>
+      <x:c r="A36" s="60"/>
       <x:c r="B36" s="13" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C36" s="30">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C36" s="28">
         <x:v>0.1178</x:v>
       </x:c>
-      <x:c r="D36" s="26">
+      <x:c r="D36" s="24">
         <x:v>0.1037</x:v>
       </x:c>
       <x:c r="E36" s="14">
@@ -3034,319 +3243,378 @@
       </x:c>
       <x:c r="G36" s="3"/>
       <x:c r="H36" s="3"/>
-      <x:c r="I36" s="42"/>
-      <x:c r="J36" s="42"/>
-      <x:c r="K36" s="42"/>
+      <x:c r="I36" s="19"/>
+      <x:c r="J36" s="19"/>
+      <x:c r="K36" s="19"/>
     </x:row>
     <x:row r="37" spans="1:11">
-      <x:c r="A37" s="42"/>
-      <x:c r="B37" s="20"/>
-      <x:c r="C37" s="20"/>
-      <x:c r="D37" s="20"/>
-      <x:c r="E37" s="20"/>
-      <x:c r="F37" s="20"/>
-      <x:c r="G37" s="20"/>
-      <x:c r="H37" s="20"/>
-      <x:c r="I37" s="42"/>
-      <x:c r="J37" s="42"/>
-      <x:c r="K37" s="42"/>
+      <x:c r="A37" s="60"/>
+      <x:c r="B37" s="19"/>
+      <x:c r="C37" s="19"/>
+      <x:c r="D37" s="19"/>
+      <x:c r="E37" s="19"/>
+      <x:c r="F37" s="19"/>
+      <x:c r="G37" s="19"/>
+      <x:c r="H37" s="19"/>
+      <x:c r="I37" s="19"/>
+      <x:c r="J37" s="19"/>
+      <x:c r="K37" s="19"/>
     </x:row>
     <x:row r="38" spans="1:11">
-      <x:c r="A38" s="42"/>
-      <x:c r="B38" s="20"/>
-      <x:c r="C38" s="38" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D38" s="20"/>
-      <x:c r="E38" s="20"/>
-      <x:c r="F38" s="20"/>
-      <x:c r="G38" s="20"/>
-      <x:c r="H38" s="20"/>
-      <x:c r="I38" s="42"/>
-      <x:c r="J38" s="42"/>
-      <x:c r="K38" s="42"/>
+      <x:c r="A38" s="60"/>
+      <x:c r="B38" s="19"/>
+      <x:c r="C38" s="36" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D38" s="19"/>
+      <x:c r="E38" s="19"/>
+      <x:c r="F38" s="19"/>
+      <x:c r="G38" s="19"/>
+      <x:c r="H38" s="19"/>
+      <x:c r="I38" s="19"/>
+      <x:c r="J38" s="19"/>
+      <x:c r="K38" s="19"/>
     </x:row>
     <x:row r="39" spans="1:11">
-      <x:c r="A39" s="42"/>
-      <x:c r="B39" s="20"/>
-      <x:c r="C39" s="35" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D39" s="20"/>
-      <x:c r="E39" s="20"/>
-      <x:c r="F39" s="20"/>
-      <x:c r="G39" s="20"/>
-      <x:c r="H39" s="20"/>
-      <x:c r="I39" s="42"/>
-      <x:c r="J39" s="42"/>
-      <x:c r="K39" s="42"/>
+      <x:c r="A39" s="60"/>
+      <x:c r="B39" s="19"/>
+      <x:c r="C39" s="33" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D39" s="19"/>
+      <x:c r="E39" s="19"/>
+      <x:c r="F39" s="19"/>
+      <x:c r="G39" s="19"/>
+      <x:c r="H39" s="19"/>
+      <x:c r="I39" s="19"/>
+      <x:c r="J39" s="19"/>
+      <x:c r="K39" s="19"/>
     </x:row>
     <x:row r="40" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A40" s="42"/>
+      <x:c r="A40" s="60"/>
       <x:c r="B40" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C40" s="7" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="I40" s="19"/>
+      <x:c r="J40" s="19"/>
+      <x:c r="K40" s="19"/>
+    </x:row>
+    <x:row r="41" spans="1:11" ht="25.85000000000000142109">
+      <x:c r="A41" s="60"/>
+      <x:c r="B41" s="8" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C41" s="10">
+        <x:v>0.89849999999999997</x:v>
+      </x:c>
+      <x:c r="I41" s="19"/>
+      <x:c r="J41" s="19"/>
+      <x:c r="K41" s="19"/>
+    </x:row>
+    <x:row r="42" spans="1:11">
+      <x:c r="A42" s="60"/>
+      <x:c r="B42" s="11" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="I40" s="42"/>
-      <x:c r="J40" s="42"/>
-      <x:c r="K40" s="42"/>
-    </x:row>
-    <x:row r="41" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A41" s="42"/>
-      <x:c r="B41" s="8" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C41" s="10">
-        <x:v>0.10150000000000001</x:v>
-      </x:c>
-      <x:c r="I41" s="42"/>
-      <x:c r="J41" s="42"/>
-      <x:c r="K41" s="42"/>
-    </x:row>
-    <x:row r="42" spans="1:11">
-      <x:c r="A42" s="42"/>
-      <x:c r="B42" s="11" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C42" s="25">
+      <x:c r="C42" s="23">
         <x:v>0.053000000000000003</x:v>
       </x:c>
-      <x:c r="I42" s="42"/>
-      <x:c r="J42" s="42"/>
-      <x:c r="K42" s="42"/>
+      <x:c r="I42" s="19"/>
+      <x:c r="J42" s="19"/>
+      <x:c r="K42" s="19"/>
     </x:row>
     <x:row r="43" spans="1:11">
-      <x:c r="A43" s="42"/>
+      <x:c r="A43" s="60"/>
       <x:c r="B43" s="11" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C43" s="25">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C43" s="23">
         <x:v>0.094999999999999996</x:v>
       </x:c>
-      <x:c r="I43" s="42"/>
-      <x:c r="J43" s="42"/>
-      <x:c r="K43" s="42"/>
+      <x:c r="I43" s="19"/>
+      <x:c r="J43" s="19"/>
+      <x:c r="K43" s="19"/>
     </x:row>
     <x:row r="44" spans="1:11">
-      <x:c r="A44" s="42"/>
+      <x:c r="A44" s="60"/>
       <x:c r="B44" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C44" s="15">
         <x:v>0.085999999999999988</x:v>
       </x:c>
-      <x:c r="I44" s="42"/>
-      <x:c r="J44" s="42"/>
-      <x:c r="K44" s="42"/>
+      <x:c r="I44" s="19"/>
+      <x:c r="J44" s="19"/>
+      <x:c r="K44" s="19"/>
     </x:row>
     <x:row r="45" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A45" s="42"/>
+      <x:c r="A45" s="60"/>
       <x:c r="B45" s="13" t="s">
-        <x:v>45</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C45" s="16">
         <x:v>0.1787</x:v>
       </x:c>
-      <x:c r="I45" s="42"/>
-      <x:c r="J45" s="42"/>
-      <x:c r="K45" s="42"/>
+      <x:c r="I45" s="19"/>
+      <x:c r="J45" s="19"/>
+      <x:c r="K45" s="19"/>
     </x:row>
     <x:row r="46" spans="1:11">
-      <x:c r="A46" s="42"/>
-      <x:c r="B46" s="42"/>
-      <x:c r="C46" s="42"/>
-      <x:c r="D46" s="42"/>
-      <x:c r="E46" s="42"/>
-      <x:c r="F46" s="42"/>
-      <x:c r="G46" s="42"/>
-      <x:c r="H46" s="42"/>
-      <x:c r="I46" s="42"/>
-      <x:c r="J46" s="42"/>
-      <x:c r="K46" s="42"/>
+      <x:c r="A46" s="60"/>
+      <x:c r="B46" s="19"/>
+      <x:c r="C46" s="19"/>
+      <x:c r="D46" s="19"/>
+      <x:c r="E46" s="19"/>
+      <x:c r="F46" s="19"/>
+      <x:c r="G46" s="19"/>
+      <x:c r="H46" s="19"/>
+      <x:c r="I46" s="19"/>
+      <x:c r="J46" s="19"/>
+      <x:c r="K46" s="19"/>
     </x:row>
     <x:row r="47" spans="1:11">
-      <x:c r="A47" s="42"/>
-      <x:c r="B47" s="42"/>
-      <x:c r="C47" s="42"/>
-      <x:c r="D47" s="42"/>
-      <x:c r="E47" s="42"/>
-      <x:c r="F47" s="42"/>
-      <x:c r="G47" s="42"/>
-      <x:c r="H47" s="42"/>
-      <x:c r="I47" s="42"/>
-      <x:c r="J47" s="42"/>
-      <x:c r="K47" s="42"/>
+      <x:c r="A47" s="60"/>
+      <x:c r="J47" s="19"/>
+      <x:c r="K47" s="19"/>
     </x:row>
     <x:row r="48" spans="1:11">
-      <x:c r="A48" s="42"/>
-      <x:c r="B48" s="42"/>
-      <x:c r="C48" s="42"/>
-      <x:c r="D48" s="42"/>
-      <x:c r="E48" s="42"/>
-      <x:c r="F48" s="42"/>
-      <x:c r="G48" s="42"/>
-      <x:c r="H48" s="42"/>
-      <x:c r="I48" s="42"/>
-      <x:c r="J48" s="42"/>
-      <x:c r="K48" s="42"/>
-    </x:row>
-    <x:row r="49" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A49" s="44"/>
-      <x:c r="B49" s="5" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C49" s="6" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D49" s="6" t="s">
+      <x:c r="A48" s="60"/>
+      <x:c r="J48" s="19"/>
+      <x:c r="K48" s="19"/>
+    </x:row>
+    <x:row r="49" spans="1:11">
+      <x:c r="A49" s="37"/>
+      <x:c r="K49" s="19"/>
+    </x:row>
+    <x:row r="50" spans="1:11">
+      <x:c r="A50" s="19"/>
+      <x:c r="K50" s="19"/>
+    </x:row>
+    <x:row r="51" spans="1:11">
+      <x:c r="A51" s="19"/>
+      <x:c r="K51" s="19"/>
+    </x:row>
+    <x:row r="52" spans="1:11">
+      <x:c r="A52" s="19"/>
+      <x:c r="K52" s="19"/>
+    </x:row>
+    <x:row r="53" spans="1:11">
+      <x:c r="A53" s="19"/>
+      <x:c r="K53" s="19"/>
+    </x:row>
+    <x:row r="54" spans="1:11">
+      <x:c r="A54" s="19"/>
+      <x:c r="K54" s="19"/>
+    </x:row>
+    <x:row r="55" spans="1:11">
+      <x:c r="A55" s="19"/>
+      <x:c r="B55" s="3"/>
+      <x:c r="C55" s="3"/>
+      <x:c r="D55" s="3"/>
+      <x:c r="E55" s="3"/>
+      <x:c r="F55" s="3"/>
+      <x:c r="G55" s="54" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="H55" s="36" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I55" s="35" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="J55" s="19"/>
+      <x:c r="K55" s="19"/>
+    </x:row>
+    <x:row r="56" spans="1:11">
+      <x:c r="A56" s="19"/>
+      <x:c r="B56" s="3"/>
+      <x:c r="C56" s="3"/>
+      <x:c r="D56" s="3"/>
+      <x:c r="E56" s="33" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F56" s="33" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G56" s="33" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="H56" s="33" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I56" s="33" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="J56" s="19"/>
+      <x:c r="K56" s="19"/>
+    </x:row>
+    <x:row r="57" spans="1:11" ht="27.85000000000000142109">
+      <x:c r="A57" s="37"/>
+      <x:c r="B57" s="55" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C57" s="6" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D57" s="6" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E57" s="6" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F57" s="6" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="G57" s="6" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H57" s="6" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="I57" s="7" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J57" s="19"/>
+      <x:c r="K57" s="19"/>
+    </x:row>
+    <x:row r="58" spans="2:9" ht="25.85000000000000142109">
+      <x:c r="B58" s="8" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E49" s="6" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F49" s="6" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="G49" s="6" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="H49" s="6" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="I49" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="K49" s="20"/>
-    </x:row>
-    <x:row r="50" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A50" s="20"/>
-      <x:c r="B50" s="8" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C50" s="49">
+      <x:c r="C58" s="42">
         <x:v>0.1115</x:v>
       </x:c>
-      <x:c r="D50" s="45"/>
-      <x:c r="E50" s="45"/>
-      <x:c r="F50" s="45"/>
-      <x:c r="G50" s="49"/>
-      <x:c r="H50" s="45"/>
-      <x:c r="I50" s="50"/>
-      <x:c r="K50" s="20"/>
-    </x:row>
-    <x:row r="51" spans="1:11">
-      <x:c r="A51" s="20"/>
-      <x:c r="B51" s="11" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C51" s="51">
+      <x:c r="D58" s="38">
+        <x:v>0.1104</x:v>
+      </x:c>
+      <x:c r="E58" s="38">
+        <x:v>0.1047</x:v>
+      </x:c>
+      <x:c r="F58" s="50">
+        <x:v>0.1003</x:v>
+      </x:c>
+      <x:c r="G58" s="44">
+        <x:v>0.097999999999999998</x:v>
+      </x:c>
+      <x:c r="H58" s="38">
+        <x:v>0.1139</x:v>
+      </x:c>
+      <x:c r="I58" s="49">
+        <x:v>0.099500000000000011</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="2:9">
+      <x:c r="B59" s="11" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C59" s="12">
         <x:v>0.061399999999999999</x:v>
       </x:c>
-      <x:c r="D51" s="12" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="E51" s="12"/>
-      <x:c r="F51" s="12"/>
-      <x:c r="G51" s="12"/>
-      <x:c r="H51" s="12"/>
-      <x:c r="I51" s="15"/>
-      <x:c r="K51" s="20"/>
-    </x:row>
-    <x:row r="52" spans="1:11">
-      <x:c r="A52" s="20"/>
-      <x:c r="B52" s="11" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C52" s="51">
+      <x:c r="D59" s="12">
+        <x:v>0.079500000000000004</x:v>
+      </x:c>
+      <x:c r="E59" s="12">
+        <x:v>0.075</x:v>
+      </x:c>
+      <x:c r="F59" s="12">
+        <x:v>0.067300000000000004</x:v>
+      </x:c>
+      <x:c r="G59" s="48">
+        <x:v>0.060699999999999998</x:v>
+      </x:c>
+      <x:c r="H59" s="47">
+        <x:v>0.057799999999999996</x:v>
+      </x:c>
+      <x:c r="I59" s="45">
+        <x:v>0.048699999999999999</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="2:9">
+      <x:c r="B60" s="11" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C60" s="12">
         <x:v>0.1021</x:v>
       </x:c>
-      <x:c r="D52" s="12"/>
-      <x:c r="E52" s="12"/>
-      <x:c r="F52" s="12"/>
-      <x:c r="G52" s="12"/>
-      <x:c r="H52" s="12"/>
-      <x:c r="I52" s="15"/>
-      <x:c r="K52" s="20"/>
-    </x:row>
-    <x:row r="53" spans="1:11">
-      <x:c r="A53" s="20"/>
-      <x:c r="B53" s="11" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C53" s="51">
+      <x:c r="D60" s="12">
+        <x:v>0.1152</x:v>
+      </x:c>
+      <x:c r="E60" s="12">
+        <x:v>0.1062</x:v>
+      </x:c>
+      <x:c r="F60" s="12">
+        <x:v>0.1065</x:v>
+      </x:c>
+      <x:c r="G60" s="43">
+        <x:v>0.098799999999999999</x:v>
+      </x:c>
+      <x:c r="H60" s="47">
+        <x:v>0.1024</x:v>
+      </x:c>
+      <x:c r="I60" s="51">
+        <x:v>0.10390000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="2:9">
+      <x:c r="B61" s="11" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C61" s="12">
         <x:v>0.13800000000000001</x:v>
       </x:c>
-      <x:c r="D53" s="12"/>
-      <x:c r="E53" s="12"/>
-      <x:c r="F53" s="12"/>
-      <x:c r="G53" s="12"/>
-      <x:c r="H53" s="12"/>
-      <x:c r="I53" s="15"/>
-      <x:c r="K53" s="20"/>
-    </x:row>
-    <x:row r="54" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A54" s="20"/>
-      <x:c r="B54" s="13" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C54" s="51">
+      <x:c r="D61" s="12">
+        <x:v>0.1065</x:v>
+      </x:c>
+      <x:c r="E61" s="12">
+        <x:v>0.1145</x:v>
+      </x:c>
+      <x:c r="F61" s="48">
+        <x:v>0.097500000000000009</x:v>
+      </x:c>
+      <x:c r="G61" s="47">
+        <x:v>0.094700000000000006</x:v>
+      </x:c>
+      <x:c r="H61" s="12">
+        <x:v>0.10589999999999999</x:v>
+      </x:c>
+      <x:c r="I61" s="45">
+        <x:v>0.079899999999999993</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="2:9" ht="17.14999999999999857891">
+      <x:c r="B62" s="13" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C62" s="53">
         <x:v>0.14849999999999999</x:v>
       </x:c>
-      <x:c r="D54" s="14"/>
-      <x:c r="E54" s="14"/>
-      <x:c r="F54" s="14"/>
-      <x:c r="G54" s="14"/>
-      <x:c r="H54" s="14"/>
-      <x:c r="I54" s="16"/>
-      <x:c r="K54" s="20"/>
-    </x:row>
-    <x:row r="55" spans="1:11">
-      <x:c r="A55" s="20"/>
-      <x:c r="B55" s="20"/>
-      <x:c r="C55" s="20"/>
-      <x:c r="D55" s="20"/>
-      <x:c r="E55" s="20"/>
-      <x:c r="F55" s="20"/>
-      <x:c r="G55" s="20"/>
-      <x:c r="H55" s="20"/>
-      <x:c r="I55" s="20"/>
-      <x:c r="J55" s="20"/>
-      <x:c r="K55" s="20"/>
-    </x:row>
-    <x:row r="56" spans="1:11">
-      <x:c r="A56" s="20"/>
-      <x:c r="B56" s="20"/>
-      <x:c r="C56" s="20"/>
-      <x:c r="D56" s="20"/>
-      <x:c r="E56" s="20"/>
-      <x:c r="F56" s="20"/>
-      <x:c r="G56" s="20"/>
-      <x:c r="H56" s="20"/>
-      <x:c r="I56" s="20"/>
-      <x:c r="J56" s="20"/>
-      <x:c r="K56" s="20"/>
-    </x:row>
-    <x:row r="57" spans="1:11">
-      <x:c r="A57" s="44"/>
-      <x:c r="B57" s="20"/>
-      <x:c r="C57" s="20"/>
-      <x:c r="D57" s="20"/>
-      <x:c r="E57" s="20"/>
-      <x:c r="F57" s="20"/>
-      <x:c r="G57" s="20"/>
-      <x:c r="H57" s="20"/>
-      <x:c r="I57" s="20"/>
-      <x:c r="J57" s="20"/>
-      <x:c r="K57" s="20"/>
+      <x:c r="D62" s="14">
+        <x:v>0.154</x:v>
+      </x:c>
+      <x:c r="E62" s="52">
+        <x:v>0.14560000000000001</x:v>
+      </x:c>
+      <x:c r="F62" s="14">
+        <x:v>0.1661</x:v>
+      </x:c>
+      <x:c r="G62" s="46">
+        <x:v>0.13389999999999999</x:v>
+      </x:c>
+      <x:c r="H62" s="14">
+        <x:v>0.16569999999999999</x:v>
+      </x:c>
+      <x:c r="I62" s="16">
+        <x:v>0.1525</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="4">
+  <x:mergeCells count="3">
     <x:mergeCell ref="A1:A3"/>
-    <x:mergeCell ref="I1:K48"/>
-    <x:mergeCell ref="B46:H48"/>
     <x:mergeCell ref="A4:A48"/>
+    <x:mergeCell ref="B11:B12"/>
   </x:mergeCells>
   <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51138889789581298828" footer="0.51138889789581298828"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>

</xml_diff>

<commit_message>
docs: Modify dics loss to score on grid search
</commit_message>
<xml_diff>
--- a/Learning record sheet.xlsx
+++ b/Learning record sheet.xlsx
@@ -19,99 +19,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">Dice Score (test)
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="7"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="7"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>동일 테스트셋 10번 테스트 평균값</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">[Double] 복합 데이터 증강
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>(Batch size = 64)</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">[Triple] 복합 데이터 증강
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>(Batch size = 64)</x:t>
-    </x:r>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+  <x:si>
+    <x:t>[이미지 사이즈]
+224 * 224</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Quad] 복합 데이터 증강</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Double] 복합 데이터 증강</x:t>
+  </x:si>
+  <x:si>
+    <x:t>동일 테스트셋
+10번 테스트 평균값</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 
+(중앙점 평행 이동)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dice Score (test)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 1 
+(1:1 비율 변환)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Original + Case 1 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Triple] 복합 데이터 증강</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 1 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 4 
+(데이터들의 최대 길이 대비 축소 비율의 평균값으로
+크기 변환, 가로/세로 비율 고정)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3rd Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1st Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2nd Performance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>train lr std</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Single] 데이터 증강</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Best Dice Score (train)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Best Dice Score (val)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Blue == 2nd (2 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Red == 1st (3 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Green == 3rd (1 point)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>best dice loss (val)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>best dice loss (train)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 2 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 3
+(비율 고정, 최대 크기 변환)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 1 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2  + Case 1 + Case 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case 2 + Case 3 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 3 + Case 4</x:t>
   </x:si>
   <x:si>
     <x:r>
@@ -145,30 +188,6 @@
     </x:r>
   </x:si>
   <x:si>
-    <x:t>Case 1 
-(1:1 비율 변환)</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Original + Case 1 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>[이미지 사이즈]
-224 * 224</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 
-(중앙점 평행 이동)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 4</x:t>
-  </x:si>
-  <x:si>
     <x:r>
       <x:t xml:space="preserve">모든 데이터 중앙 평행이동
 </x:t>
@@ -200,102 +219,19 @@
     </x:r>
   </x:si>
   <x:si>
-    <x:r>
-      <x:t xml:space="preserve">[Single] 데이터 증강
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>(Batch size = 64)</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">[Quad] 복합 데이터 증강
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>(Batch size = 64)</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 2 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blue == 2nd (2 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Red == 1st (3 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Green == 3rd (1 point)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>best dice loss (train)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Best Dice Score (train)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Best Dice Score (val)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>best dice loss (val)</x:t>
+    <x:t>val lr std</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 치환</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 Point</x:t>
   </x:si>
   <x:si>
     <x:t>4 Point</x:t>
@@ -304,127 +240,27 @@
     <x:t>2 Point</x:t>
   </x:si>
   <x:si>
+    <x:t>9 Point</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 Point</x:t>
+  </x:si>
+  <x:si>
     <x:t>3 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2nd Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>train lr std</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1st Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3rd Performance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 4 
-(데이터들의 최대 길이 대비 축소 비율의 평균값으로
-크기 변환, 가로/세로 비율 고정)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 2 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 2 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2 + Case 1 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 3
-(비율 고정, 최대 크기 변환)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Case 2  + Case 1 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 3 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original + Case 1 + Case 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 Point</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original</x:t>
-  </x:si>
-  <x:si>
-    <x:t>val lr std</x:t>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve">데이터 치환
-</x:t>
-    </x:r>
-    <x:r>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-          <x:rPr hs:extension="1">
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-            <hs:size val="100"/>
-            <hs:ratio val="100"/>
-            <hs:spacing val="0"/>
-            <hs:offset val="0"/>
-          </x:rPr>
-        </mc:Choice>
-        <mc:Fallback>
-          <x:rPr>
-            <x:rFont val="맑은 고딕"/>
-            <x:sz val="8"/>
-            <x:color rgb="ffbfbfbf"/>
-            <x:b val="1"/>
-          </x:rPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <x:t>(Batch size = 64)</x:t>
-    </x:r>
   </x:si>
   <x:si>
     <x:t>Grid Search Start
 (Dice Score (test))</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original + Case 1 + Case 2 + Case 3 + Case 4</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="20">
+  <x:fonts count="19">
     <x:font>
       <x:name val="맑은 고딕"/>
       <x:sz val="11"/>
@@ -613,7 +449,7 @@
         <x:font hs:extension="1">
           <x:name val="맑은 고딕"/>
           <x:sz val="7"/>
-          <x:color rgb="ffbfbfbf"/>
+          <x:color rgb="ffffffff"/>
           <x:b val="1"/>
           <hs:size val="100"/>
           <hs:ratio val="100"/>
@@ -625,7 +461,7 @@
         <x:font>
           <x:name val="맑은 고딕"/>
           <x:sz val="7"/>
-          <x:color rgb="ffbfbfbf"/>
+          <x:color rgb="ffffffff"/>
           <x:b val="1"/>
         </x:font>
       </mc:Fallback>
@@ -648,28 +484,6 @@
           <x:name val="맑은 고딕"/>
           <x:sz val="8"/>
           <x:color rgb="ffbfbfbf"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="7"/>
-          <x:color rgb="ffffffff"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="7"/>
-          <x:color rgb="ffffffff"/>
           <x:b val="1"/>
         </x:font>
       </mc:Fallback>
@@ -885,7 +699,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="69">
+  <x:cellXfs count="70">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -1579,6 +1393,123 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="top" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="top" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="top" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="top" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -1593,103 +1524,6 @@
     <x:xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
@@ -1700,6 +1534,19 @@
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -2110,24 +1957,612 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart0.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:rPr>
+              <a:t>[Single] 데이터 증강</a:t>
+            </a:r>
+            <a:endParaRPr/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dice Score (test)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$13:$F$13</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v xml:space="preserve">Original + Case 1 </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original + Case 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Original + Case 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Original + Case 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>G/표준</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.8912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8773</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="231356873"/>
+        <c:axId val="507462935"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="231356873"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:crossAx val="507462935"/>
+        <c:delete val="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="507462935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:crossAx val="231356873"/>
+        <c:delete val="0"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="G/표준" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+    <a:p>
+      <a:pPr algn="l">
+        <a:defRPr sz="1000" b="0" i="0" u="none">
+          <a:latin typeface="Calibri"/>
+          <a:ea typeface="맑은 고딕"/>
+          <a:cs typeface="맑은 고딕"/>
+          <a:sym typeface="맑은 고딕"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext uri="CC8EB2C9-7E31-499d-B8F2-F6CE61031016">
+      <ho:hncChartStyle xmlns:ho="http://schemas.haansoft.com/office/8.0" layoutIndex="-1" colorIndex="0" styleIndex="0"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:rPr>
+              <a:t>[Double] 복합 데이터 증강</a:t>
+            </a:r>
+            <a:endParaRPr/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dice Score (test)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$22:$H$22</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Original + Case 1 + Case 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original + Case 1 + Case 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Original + Case 1 + Case 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Original + Case 2 + Case 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Original + Case 2 + Case 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Original + Case 3 + Case 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>G/표준</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.9048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8906</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9029</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8924</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8877</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="239808173"/>
+        <c:axId val="581027553"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="239808173"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:crossAx val="581027553"/>
+        <c:delete val="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="581027553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:crossAx val="239808173"/>
+        <c:delete val="0"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="G/표준" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+    <a:p>
+      <a:pPr algn="l">
+        <a:defRPr sz="1000" b="0" i="0" u="none">
+          <a:latin typeface="Calibri"/>
+          <a:ea typeface="맑은 고딕"/>
+          <a:cs typeface="맑은 고딕"/>
+          <a:sym typeface="맑은 고딕"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext uri="CC8EB2C9-7E31-499d-B8F2-F6CE61031016">
+      <ho:hncChartStyle xmlns:ho="http://schemas.haansoft.com/office/8.0" layoutIndex="-1" colorIndex="0" styleIndex="0"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" i="0" u="none">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="맑은 고딕"/>
+                <a:cs typeface="맑은 고딕"/>
+                <a:sym typeface="맑은 고딕"/>
+              </a:rPr>
+              <a:t>[Triple] 복합 데이터 증강</a:t>
+            </a:r>
+            <a:endParaRPr/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dice Score (test)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$31:$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Original + Case 1 + Case 2 + Case 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original + Case 1 + Case 2 + Case 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Original + Case 1 + Case 3 + Case 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Original + Case 2 + Case 3 + Case 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>G/표준</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.9001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8965</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.894</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="247092664"/>
+        <c:axId val="657964723"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="247092664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:crossAx val="657964723"/>
+        <c:delete val="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="657964723"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:crossAx val="247092664"/>
+        <c:delete val="0"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="G/표준" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+    <a:p>
+      <a:pPr algn="l">
+        <a:defRPr sz="1000" b="0" i="0" u="none">
+          <a:latin typeface="Calibri"/>
+          <a:ea typeface="맑은 고딕"/>
+          <a:cs typeface="맑은 고딕"/>
+          <a:sym typeface="맑은 고딕"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext uri="CC8EB2C9-7E31-499d-B8F2-F6CE61031016">
+      <ho:hncChartStyle xmlns:ho="http://schemas.haansoft.com/office/8.0" layoutIndex="-1" colorIndex="0" styleIndex="0"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing0.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="" fPublished="0">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="9" name="그림 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2140,14 +2575,110 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17757322" y="625928"/>
-          <a:ext cx="4680857" cy="3673928"/>
+          <a:off x="17770930" y="136071"/>
+          <a:ext cx="3061607" cy="2381250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame fPublished="0">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="차트 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="14301107" y="2639785"/>
+        <a:ext cx="4313464" cy="2585357"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame fPublished="0">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="차트 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="19648714" y="4259035"/>
+        <a:ext cx="5905500" cy="3565071"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1895475</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame fPublished="0">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="차트 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="14301107" y="7320643"/>
+        <a:ext cx="5334000" cy="3224893"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2468,8 +2999,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:K62"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <x:selection activeCell="C23" activeCellId="0" sqref="C23:C23"/>
+    <x:sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <x:selection activeCell="D34" activeCellId="0" sqref="D34:D34"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
@@ -2487,11 +3018,11 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:11">
-      <x:c r="A1" s="57" t="s">
-        <x:v>6</x:v>
+      <x:c r="A1" s="66" t="s">
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="31" t="s">
-        <x:v>20</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C1" s="3"/>
       <x:c r="D1" s="3"/>
@@ -2504,9 +3035,9 @@
       <x:c r="K1" s="19"/>
     </x:row>
     <x:row r="2" spans="1:11">
-      <x:c r="A2" s="58"/>
+      <x:c r="A2" s="67"/>
       <x:c r="B2" s="30" t="s">
-        <x:v>19</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C2" s="3"/>
       <x:c r="D2" s="3"/>
@@ -2519,9 +3050,9 @@
       <x:c r="K2" s="19"/>
     </x:row>
     <x:row r="3" spans="1:11">
-      <x:c r="A3" s="58"/>
+      <x:c r="A3" s="67"/>
       <x:c r="B3" s="29" t="s">
-        <x:v>21</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C3" s="3"/>
       <x:c r="D3" s="3"/>
@@ -2534,34 +3065,36 @@
       <x:c r="K3" s="19"/>
     </x:row>
     <x:row r="4" spans="1:11" ht="55.5" customHeight="1">
-      <x:c r="A4" s="59"/>
+      <x:c r="A4" s="3"/>
       <x:c r="B4" s="5" t="s">
-        <x:v>54</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C4" s="6" t="s">
-        <x:v>52</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D4" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F4" s="6" t="s">
-        <x:v>45</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G4" s="56" t="s">
-        <x:v>39</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H4"/>
       <x:c r="I4" s="19"/>
       <x:c r="J4" s="19"/>
       <x:c r="K4" s="19"/>
     </x:row>
-    <x:row r="5" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A5" s="59"/>
+    <x:row r="5" spans="1:11" ht="32.75">
+      <x:c r="A5" s="63" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="B5" s="8" t="s">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="9">
         <x:v>0.86950000000000005</x:v>
@@ -2583,12 +3116,12 @@
       <x:c r="K5" s="19"/>
     </x:row>
     <x:row r="6" spans="1:11">
-      <x:c r="A6" s="59"/>
+      <x:c r="A6" s="3"/>
       <x:c r="B6" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C6" s="12">
-        <x:v>0.096600000000000008</x:v>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C6" s="64">
+        <x:v>0.90039999999999998</x:v>
       </x:c>
       <x:c r="D6" s="12">
         <x:v>0.0876</x:v>
@@ -2607,12 +3140,12 @@
       <x:c r="K6" s="19"/>
     </x:row>
     <x:row r="7" spans="1:11">
-      <x:c r="A7" s="59"/>
+      <x:c r="A7" s="3"/>
       <x:c r="B7" s="11" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C7" s="12">
-        <x:v>0.1231</x:v>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C7" s="64">
+        <x:v>0.87690000000000001</x:v>
       </x:c>
       <x:c r="D7" s="12">
         <x:v>0.13109999999999999</x:v>
@@ -2631,9 +3164,9 @@
       <x:c r="K7" s="19"/>
     </x:row>
     <x:row r="8" spans="1:11">
-      <x:c r="A8" s="59"/>
+      <x:c r="A8" s="3"/>
       <x:c r="B8" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C8" s="12">
         <x:v>0.21510000000000001</x:v>
@@ -2655,9 +3188,9 @@
       <x:c r="K8" s="19"/>
     </x:row>
     <x:row r="9" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A9" s="59"/>
+      <x:c r="A9" s="3"/>
       <x:c r="B9" s="13" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C9" s="14">
         <x:v>0.2475</x:v>
@@ -2679,7 +3212,7 @@
       <x:c r="K9" s="19"/>
     </x:row>
     <x:row r="10" spans="1:11">
-      <x:c r="A10" s="60"/>
+      <x:c r="A10" s="19"/>
       <x:c r="B10" s="3"/>
       <x:c r="C10" s="19"/>
       <x:c r="D10" s="19"/>
@@ -2692,7 +3225,7 @@
       <x:c r="K10" s="19"/>
     </x:row>
     <x:row r="11" spans="1:11">
-      <x:c r="A11" s="60"/>
+      <x:c r="A11" s="19"/>
       <x:c r="B11" s="68" t="s">
         <x:v>55</x:v>
       </x:c>
@@ -2707,8 +3240,8 @@
       <x:c r="K11" s="19"/>
     </x:row>
     <x:row r="12" spans="1:11">
-      <x:c r="A12" s="60"/>
-      <x:c r="B12" s="67"/>
+      <x:c r="A12" s="19"/>
+      <x:c r="B12" s="69"/>
       <x:c r="C12" s="19"/>
       <x:c r="D12" s="19"/>
       <x:c r="E12" s="3"/>
@@ -2719,37 +3252,39 @@
       <x:c r="J12" s="19"/>
       <x:c r="K12" s="19"/>
     </x:row>
-    <x:row r="13" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A13" s="60"/>
+    <x:row r="13" spans="1:11" ht="17.14999999999999857891">
+      <x:c r="A13" s="19"/>
       <x:c r="B13" s="5" t="s">
-        <x:v>12</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C13" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D13" s="61" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D13" s="57" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E13" s="6" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F13" s="7" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="E13" s="6" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="F13" s="7" t="s">
-        <x:v>10</x:v>
       </x:c>
       <x:c r="G13" s="2"/>
       <x:c r="I13" s="19"/>
       <x:c r="J13" s="19"/>
       <x:c r="K13" s="19"/>
     </x:row>
-    <x:row r="14" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A14" s="60"/>
+    <x:row r="14" spans="1:11" ht="32.75">
+      <x:c r="A14" s="63" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="B14" s="8" t="s">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C14" s="9">
         <x:v>0.89119999999999999</x:v>
       </x:c>
-      <x:c r="D14" s="62">
+      <x:c r="D14" s="58">
         <x:v>0.89970000000000006</x:v>
       </x:c>
       <x:c r="E14" s="9">
@@ -2764,21 +3299,21 @@
       <x:c r="K14" s="19"/>
     </x:row>
     <x:row r="15" spans="1:11">
-      <x:c r="A15" s="60"/>
+      <x:c r="A15" s="19"/>
       <x:c r="B15" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C15" s="12">
-        <x:v>0.064600000000000002</x:v>
-      </x:c>
-      <x:c r="D15" s="63">
-        <x:v>0.054699999999999993</x:v>
-      </x:c>
-      <x:c r="E15" s="12">
-        <x:v>0.082400000000000007</x:v>
-      </x:c>
-      <x:c r="F15" s="15">
-        <x:v>0.079299999999999993</x:v>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C15" s="64">
+        <x:v>0.93540000000000001</x:v>
+      </x:c>
+      <x:c r="D15" s="65">
+        <x:v>0.94530000000000003</x:v>
+      </x:c>
+      <x:c r="E15" s="64">
+        <x:v>0.91759999999999997</x:v>
+      </x:c>
+      <x:c r="F15" s="64">
+        <x:v>0.92069999999999996</x:v>
       </x:c>
       <x:c r="G15" s="3"/>
       <x:c r="I15" s="19"/>
@@ -2786,21 +3321,21 @@
       <x:c r="K15" s="19"/>
     </x:row>
     <x:row r="16" spans="1:11">
-      <x:c r="A16" s="60"/>
+      <x:c r="A16" s="19"/>
       <x:c r="B16" s="11" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C16" s="12">
-        <x:v>0.1027</x:v>
-      </x:c>
-      <x:c r="D16" s="63">
-        <x:v>0.097199999999999998</x:v>
-      </x:c>
-      <x:c r="E16" s="12">
-        <x:v>0.1116</x:v>
-      </x:c>
-      <x:c r="F16" s="15">
-        <x:v>0.10730000000000001</x:v>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C16" s="64">
+        <x:v>0.89729999999999999</x:v>
+      </x:c>
+      <x:c r="D16" s="65">
+        <x:v>0.90280000000000005</x:v>
+      </x:c>
+      <x:c r="E16" s="64">
+        <x:v>0.88839999999999997</x:v>
+      </x:c>
+      <x:c r="F16" s="64">
+        <x:v>0.89270000000000005</x:v>
       </x:c>
       <x:c r="G16" s="3"/>
       <x:c r="I16" s="19"/>
@@ -2808,14 +3343,14 @@
       <x:c r="K16" s="19"/>
     </x:row>
     <x:row r="17" spans="1:11">
-      <x:c r="A17" s="60"/>
+      <x:c r="A17" s="19"/>
       <x:c r="B17" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C17" s="12">
         <x:v>0.12130000000000001</x:v>
       </x:c>
-      <x:c r="D17" s="63">
+      <x:c r="D17" s="59">
         <x:v>0.14050000000000001</x:v>
       </x:c>
       <x:c r="E17" s="12">
@@ -2830,14 +3365,14 @@
       <x:c r="K17" s="19"/>
     </x:row>
     <x:row r="18" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A18" s="60"/>
+      <x:c r="A18" s="19"/>
       <x:c r="B18" s="13" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C18" s="14">
         <x:v>0.16139999999999999</x:v>
       </x:c>
-      <x:c r="D18" s="64">
+      <x:c r="D18" s="60">
         <x:v>0.1817</x:v>
       </x:c>
       <x:c r="E18" s="14">
@@ -2852,7 +3387,7 @@
       <x:c r="K18" s="19"/>
     </x:row>
     <x:row r="19" spans="1:11">
-      <x:c r="A19" s="60"/>
+      <x:c r="A19" s="19"/>
       <x:c r="B19" s="19"/>
       <x:c r="C19" s="19"/>
       <x:c r="D19" s="19"/>
@@ -2865,13 +3400,13 @@
       <x:c r="K19" s="19"/>
     </x:row>
     <x:row r="20" spans="1:11">
-      <x:c r="A20" s="60"/>
+      <x:c r="A20" s="19"/>
       <x:c r="B20" s="19"/>
       <x:c r="C20" s="34" t="s">
-        <x:v>36</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D20" s="35" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E20" s="19"/>
       <x:c r="F20" s="19"/>
@@ -2882,16 +3417,16 @@
       <x:c r="K20" s="19"/>
     </x:row>
     <x:row r="21" spans="1:11">
-      <x:c r="A21" s="60"/>
+      <x:c r="A21" s="19"/>
       <x:c r="B21" s="19"/>
       <x:c r="C21" s="32" t="s">
-        <x:v>29</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D21" s="33" t="s">
-        <x:v>31</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E21" s="33" t="s">
-        <x:v>27</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F21" s="19"/>
       <x:c r="G21" s="19"/>
@@ -2900,39 +3435,41 @@
       <x:c r="J21" s="19"/>
       <x:c r="K21" s="19"/>
     </x:row>
-    <x:row r="22" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A22" s="60"/>
+    <x:row r="22" spans="1:11" ht="17.14999999999999857891">
+      <x:c r="A22" s="19"/>
       <x:c r="B22" s="5" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C22" s="61" t="s">
-        <x:v>46</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C22" s="57" t="s">
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D22" s="6" t="s">
-        <x:v>48</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E22" s="6" t="s">
-        <x:v>50</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F22" s="6" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G22" s="6" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H22" s="7" t="s">
         <x:v>42</x:v>
-      </x:c>
-      <x:c r="G22" s="6" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="H22" s="7" t="s">
-        <x:v>49</x:v>
       </x:c>
       <x:c r="I22" s="19"/>
       <x:c r="J22" s="19"/>
       <x:c r="K22" s="19"/>
     </x:row>
-    <x:row r="23" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A23" s="60"/>
+    <x:row r="23" spans="1:11" ht="32.75">
+      <x:c r="A23" s="63" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="B23" s="8" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C23" s="65">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C23" s="61">
         <x:v>0.90480000000000005</x:v>
       </x:c>
       <x:c r="D23" s="9">
@@ -2955,11 +3492,11 @@
       <x:c r="K23" s="19"/>
     </x:row>
     <x:row r="24" spans="1:11">
-      <x:c r="A24" s="60"/>
+      <x:c r="A24" s="19"/>
       <x:c r="B24" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C24" s="66">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C24" s="62">
         <x:v>0.049199999999999999</x:v>
       </x:c>
       <x:c r="D24" s="12">
@@ -2982,11 +3519,11 @@
       <x:c r="K24" s="19"/>
     </x:row>
     <x:row r="25" spans="1:11">
-      <x:c r="A25" s="60"/>
+      <x:c r="A25" s="19"/>
       <x:c r="B25" s="11" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C25" s="66">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C25" s="62">
         <x:v>0.093999999999999995</x:v>
       </x:c>
       <x:c r="D25" s="27">
@@ -3009,11 +3546,11 @@
       <x:c r="K25" s="19"/>
     </x:row>
     <x:row r="26" spans="1:11">
-      <x:c r="A26" s="60"/>
+      <x:c r="A26" s="19"/>
       <x:c r="B26" s="11" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C26" s="63">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C26" s="59">
         <x:v>0.1085</x:v>
       </x:c>
       <x:c r="D26" s="20">
@@ -3036,11 +3573,11 @@
       <x:c r="K26" s="19"/>
     </x:row>
     <x:row r="27" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A27" s="60"/>
+      <x:c r="A27" s="19"/>
       <x:c r="B27" s="13" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C27" s="64">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C27" s="60">
         <x:v>0.1237</x:v>
       </x:c>
       <x:c r="D27" s="21">
@@ -3063,7 +3600,7 @@
       <x:c r="K27" s="19"/>
     </x:row>
     <x:row r="28" spans="1:11">
-      <x:c r="A28" s="60"/>
+      <x:c r="A28" s="19"/>
       <x:c r="B28" s="19"/>
       <x:c r="C28" s="19"/>
       <x:c r="D28" s="19"/>
@@ -3076,7 +3613,7 @@
       <x:c r="K28" s="19"/>
     </x:row>
     <x:row r="29" spans="1:11">
-      <x:c r="A29" s="60"/>
+      <x:c r="A29" s="19"/>
       <x:c r="B29" s="19"/>
       <x:c r="C29" s="19"/>
       <x:c r="D29" s="19"/>
@@ -3089,19 +3626,19 @@
       <x:c r="K29" s="19"/>
     </x:row>
     <x:row r="30" spans="1:11">
-      <x:c r="A30" s="60"/>
+      <x:c r="A30" s="19"/>
       <x:c r="B30" s="19"/>
       <x:c r="C30" s="33" t="s">
-        <x:v>30</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D30" s="33" t="s">
-        <x:v>28</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E30" s="33" t="s">
-        <x:v>28</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F30" s="33" t="s">
-        <x:v>27</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G30" s="19"/>
       <x:c r="H30" s="19"/>
@@ -3110,21 +3647,21 @@
       <x:c r="K30" s="19"/>
     </x:row>
     <x:row r="31" spans="1:11" ht="28.30000000000000071054" customHeight="1">
-      <x:c r="A31" s="60"/>
+      <x:c r="A31" s="19"/>
       <x:c r="B31" s="5" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C31" s="6" t="s">
-        <x:v>18</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D31" s="6" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E31" s="6" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="F31" s="7" t="s">
-        <x:v>16</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G31" s="4"/>
       <x:c r="H31" s="4"/>
@@ -3132,10 +3669,12 @@
       <x:c r="J31" s="19"/>
       <x:c r="K31" s="19"/>
     </x:row>
-    <x:row r="32" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A32" s="60"/>
+    <x:row r="32" spans="1:11" ht="32.75">
+      <x:c r="A32" s="63" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="B32" s="8" t="s">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C32" s="9">
         <x:v>0.90010000000000001</x:v>
@@ -3156,15 +3695,15 @@
       <x:c r="K32" s="19"/>
     </x:row>
     <x:row r="33" spans="1:11">
-      <x:c r="A33" s="60"/>
+      <x:c r="A33" s="19"/>
       <x:c r="B33" s="11" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C33" s="12">
-        <x:v>0.064000000000000001</x:v>
+        <x:v>0.93600000000000005</x:v>
       </x:c>
       <x:c r="D33" s="12">
-        <x:v>0.056399999999999995</x:v>
+        <x:v>0.94359999999999999</x:v>
       </x:c>
       <x:c r="E33" s="39">
         <x:v>0.053900000000000003</x:v>
@@ -3179,15 +3718,15 @@
       <x:c r="K33" s="19"/>
     </x:row>
     <x:row r="34" spans="1:11">
-      <x:c r="A34" s="60"/>
+      <x:c r="A34" s="19"/>
       <x:c r="B34" s="11" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C34" s="12">
-        <x:v>0.099399999999999999</x:v>
+        <x:v>0.90059999999999996</x:v>
       </x:c>
       <x:c r="D34" s="12">
-        <x:v>0.098799999999999999</x:v>
+        <x:v>0.9012</x:v>
       </x:c>
       <x:c r="E34" s="12">
         <x:v>0.099199999999999999</x:v>
@@ -3202,9 +3741,9 @@
       <x:c r="K34" s="19"/>
     </x:row>
     <x:row r="35" spans="1:11">
-      <x:c r="A35" s="60"/>
+      <x:c r="A35" s="19"/>
       <x:c r="B35" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C35" s="12">
         <x:v>0.098299999999999998</x:v>
@@ -3225,9 +3764,9 @@
       <x:c r="K35" s="19"/>
     </x:row>
     <x:row r="36" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A36" s="60"/>
+      <x:c r="A36" s="19"/>
       <x:c r="B36" s="13" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C36" s="28">
         <x:v>0.1178</x:v>
@@ -3248,7 +3787,7 @@
       <x:c r="K36" s="19"/>
     </x:row>
     <x:row r="37" spans="1:11">
-      <x:c r="A37" s="60"/>
+      <x:c r="A37" s="19"/>
       <x:c r="B37" s="19"/>
       <x:c r="C37" s="19"/>
       <x:c r="D37" s="19"/>
@@ -3261,10 +3800,10 @@
       <x:c r="K37" s="19"/>
     </x:row>
     <x:row r="38" spans="1:11">
-      <x:c r="A38" s="60"/>
+      <x:c r="A38" s="19"/>
       <x:c r="B38" s="19"/>
       <x:c r="C38" s="36" t="s">
-        <x:v>37</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D38" s="19"/>
       <x:c r="E38" s="19"/>
@@ -3276,10 +3815,10 @@
       <x:c r="K38" s="19"/>
     </x:row>
     <x:row r="39" spans="1:11">
-      <x:c r="A39" s="60"/>
+      <x:c r="A39" s="19"/>
       <x:c r="B39" s="19"/>
       <x:c r="C39" s="33" t="s">
-        <x:v>26</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D39" s="19"/>
       <x:c r="E39" s="19"/>
@@ -3290,22 +3829,24 @@
       <x:c r="J39" s="19"/>
       <x:c r="K39" s="19"/>
     </x:row>
-    <x:row r="40" spans="1:11" ht="27.85000000000000142109">
-      <x:c r="A40" s="60"/>
+    <x:row r="40" spans="1:11" ht="17.14999999999999857891">
+      <x:c r="A40" s="19"/>
       <x:c r="B40" s="5" t="s">
-        <x:v>13</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C40" s="7" t="s">
-        <x:v>40</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="I40" s="19"/>
       <x:c r="J40" s="19"/>
       <x:c r="K40" s="19"/>
     </x:row>
-    <x:row r="41" spans="1:11" ht="25.85000000000000142109">
-      <x:c r="A41" s="60"/>
+    <x:row r="41" spans="1:11" ht="32.75">
+      <x:c r="A41" s="63" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="B41" s="8" t="s">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C41" s="10">
         <x:v>0.89849999999999997</x:v>
@@ -3315,9 +3856,9 @@
       <x:c r="K41" s="19"/>
     </x:row>
     <x:row r="42" spans="1:11">
-      <x:c r="A42" s="60"/>
+      <x:c r="A42" s="19"/>
       <x:c r="B42" s="11" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C42" s="23">
         <x:v>0.053000000000000003</x:v>
@@ -3327,9 +3868,9 @@
       <x:c r="K42" s="19"/>
     </x:row>
     <x:row r="43" spans="1:11">
-      <x:c r="A43" s="60"/>
+      <x:c r="A43" s="19"/>
       <x:c r="B43" s="11" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C43" s="23">
         <x:v>0.094999999999999996</x:v>
@@ -3339,9 +3880,9 @@
       <x:c r="K43" s="19"/>
     </x:row>
     <x:row r="44" spans="1:11">
-      <x:c r="A44" s="60"/>
+      <x:c r="A44" s="19"/>
       <x:c r="B44" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C44" s="15">
         <x:v>0.085999999999999988</x:v>
@@ -3351,9 +3892,9 @@
       <x:c r="K44" s="19"/>
     </x:row>
     <x:row r="45" spans="1:11" ht="17.14999999999999857891">
-      <x:c r="A45" s="60"/>
+      <x:c r="A45" s="19"/>
       <x:c r="B45" s="13" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C45" s="16">
         <x:v>0.1787</x:v>
@@ -3363,7 +3904,7 @@
       <x:c r="K45" s="19"/>
     </x:row>
     <x:row r="46" spans="1:11">
-      <x:c r="A46" s="60"/>
+      <x:c r="A46" s="19"/>
       <x:c r="B46" s="19"/>
       <x:c r="C46" s="19"/>
       <x:c r="D46" s="19"/>
@@ -3376,12 +3917,12 @@
       <x:c r="K46" s="19"/>
     </x:row>
     <x:row r="47" spans="1:11">
-      <x:c r="A47" s="60"/>
+      <x:c r="A47" s="19"/>
       <x:c r="J47" s="19"/>
       <x:c r="K47" s="19"/>
     </x:row>
     <x:row r="48" spans="1:11">
-      <x:c r="A48" s="60"/>
+      <x:c r="A48" s="19"/>
       <x:c r="J48" s="19"/>
       <x:c r="K48" s="19"/>
     </x:row>
@@ -3417,13 +3958,13 @@
       <x:c r="E55" s="3"/>
       <x:c r="F55" s="3"/>
       <x:c r="G55" s="54" t="s">
-        <x:v>36</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H55" s="36" t="s">
-        <x:v>37</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="I55" s="35" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J55" s="19"/>
       <x:c r="K55" s="19"/>
@@ -3434,19 +3975,19 @@
       <x:c r="C56" s="3"/>
       <x:c r="D56" s="3"/>
       <x:c r="E56" s="33" t="s">
-        <x:v>27</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F56" s="33" t="s">
-        <x:v>27</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G56" s="33" t="s">
-        <x:v>51</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="H56" s="33" t="s">
-        <x:v>26</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="I56" s="33" t="s">
-        <x:v>29</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="J56" s="19"/>
       <x:c r="K56" s="19"/>
@@ -3454,25 +3995,25 @@
     <x:row r="57" spans="1:11" ht="27.85000000000000142109">
       <x:c r="A57" s="37"/>
       <x:c r="B57" s="55" t="s">
-        <x:v>11</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C57" s="6" t="s">
-        <x:v>38</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D57" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E57" s="6" t="s">
-        <x:v>35</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F57" s="6" t="s">
-        <x:v>47</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G57" s="6" t="s">
-        <x:v>44</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="H57" s="6" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="I57" s="7" t="s">
         <x:v>15</x:v>
@@ -3482,7 +4023,7 @@
     </x:row>
     <x:row r="58" spans="2:9" ht="25.85000000000000142109">
       <x:c r="B58" s="8" t="s">
-        <x:v>3</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C58" s="42">
         <x:v>0.1115</x:v>
@@ -3508,7 +4049,7 @@
     </x:row>
     <x:row r="59" spans="2:9">
       <x:c r="B59" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C59" s="12">
         <x:v>0.061399999999999999</x:v>
@@ -3534,7 +4075,7 @@
     </x:row>
     <x:row r="60" spans="2:9">
       <x:c r="B60" s="11" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C60" s="12">
         <x:v>0.1021</x:v>
@@ -3560,7 +4101,7 @@
     </x:row>
     <x:row r="61" spans="2:9">
       <x:c r="B61" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C61" s="12">
         <x:v>0.13800000000000001</x:v>
@@ -3586,7 +4127,7 @@
     </x:row>
     <x:row r="62" spans="2:9" ht="17.14999999999999857891">
       <x:c r="B62" s="13" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C62" s="53">
         <x:v>0.14849999999999999</x:v>
@@ -3611,9 +4152,8 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="3">
+  <x:mergeCells count="2">
     <x:mergeCell ref="A1:A3"/>
-    <x:mergeCell ref="A4:A48"/>
     <x:mergeCell ref="B11:B12"/>
   </x:mergeCells>
   <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51138889789581298828" footer="0.51138889789581298828"/>

</xml_diff>